<commit_message>
arreglo leer excel y manipulacion datos
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\cursos\asw\LoadUsers\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -32,9 +28,6 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>Mesa</t>
-  </si>
-  <si>
     <t>NIF</t>
   </si>
   <si>
@@ -54,6 +47,18 @@
   </si>
   <si>
     <t>09940449X</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email3</t>
+  </si>
+  <si>
+    <t>email1</t>
+  </si>
+  <si>
+    <t>email2</t>
   </si>
 </sst>
 </file>
@@ -375,7 +380,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,55 +393,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>234</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="D3">
         <v>345</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+      <c r="D4">
         <v>456</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadida Validacion de correo
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>UO230766@uniovi.es</t>
+  </si>
+  <si>
+    <t>Victor Retortillo</t>
+  </si>
+  <si>
+    <t>41310533A</t>
+  </si>
+  <si>
+    <t>victor@email.</t>
   </si>
 </sst>
 </file>
@@ -397,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,14 +488,29 @@
         <v>256</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadida mas documentacion y ampliada la BBDD
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="5910"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9780" windowHeight="5415"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Nombre</t>
   </si>
@@ -77,13 +77,166 @@
   </si>
   <si>
     <t>victor@email.</t>
+  </si>
+  <si>
+    <t>Pancho Jimenez</t>
+  </si>
+  <si>
+    <t>12345678W</t>
+  </si>
+  <si>
+    <t>arrobagmail.com</t>
+  </si>
+  <si>
+    <t>Tiburcio Perez</t>
+  </si>
+  <si>
+    <t>87654321W</t>
+  </si>
+  <si>
+    <t>eltibu@email.com</t>
+  </si>
+  <si>
+    <t>Miguel Llano</t>
+  </si>
+  <si>
+    <t>61923982R</t>
+  </si>
+  <si>
+    <t>llano@mail.com</t>
+  </si>
+  <si>
+    <t>Javier Ignacio Molina</t>
+  </si>
+  <si>
+    <t>02710830G</t>
+  </si>
+  <si>
+    <t>molina.com</t>
+  </si>
+  <si>
+    <t>Sixto Naranjo Marín</t>
+  </si>
+  <si>
+    <t>77631962Q</t>
+  </si>
+  <si>
+    <t>sixton@email.com</t>
+  </si>
+  <si>
+    <t>Oscar Darío Murillo</t>
+  </si>
+  <si>
+    <t>54811130Z</t>
+  </si>
+  <si>
+    <t>murillo@email.com</t>
+  </si>
+  <si>
+    <t>Arturo Tabares</t>
+  </si>
+  <si>
+    <t>44788410G</t>
+  </si>
+  <si>
+    <t>searturo@email.com</t>
+  </si>
+  <si>
+    <t>Gabriel Jaime Jiménez</t>
+  </si>
+  <si>
+    <t>22965185F</t>
+  </si>
+  <si>
+    <t>gbj@email.com</t>
+  </si>
+  <si>
+    <t>Bernardo Posada Vera</t>
+  </si>
+  <si>
+    <t>99352012Q</t>
+  </si>
+  <si>
+    <t>berni@gmail.com</t>
+  </si>
+  <si>
+    <t>Luis Guillermo Vélez Osorio</t>
+  </si>
+  <si>
+    <t>04828404Z</t>
+  </si>
+  <si>
+    <t>lsgh@.com</t>
+  </si>
+  <si>
+    <t>Horacio Augusto Moreno Correa</t>
+  </si>
+  <si>
+    <t>56830428G</t>
+  </si>
+  <si>
+    <t>a@.com.es</t>
+  </si>
+  <si>
+    <t>Alejandro Alzate Garcés</t>
+  </si>
+  <si>
+    <t>66051967S</t>
+  </si>
+  <si>
+    <t>alex@email.com</t>
+  </si>
+  <si>
+    <t>Gustavo Hernán Rodríguez Vallejo</t>
+  </si>
+  <si>
+    <t>41998336Z</t>
+  </si>
+  <si>
+    <t>gsss@email.com</t>
+  </si>
+  <si>
+    <t>Beatriz Elena Puerta</t>
+  </si>
+  <si>
+    <t>05164173Y</t>
+  </si>
+  <si>
+    <t>puertadoor@gmail.com</t>
+  </si>
+  <si>
+    <t>Álvaro de Jesús</t>
+  </si>
+  <si>
+    <t>10797551V</t>
+  </si>
+  <si>
+    <t>jesuuuuh@mail.com</t>
+  </si>
+  <si>
+    <t>Héctor Darío Bermúdez</t>
+  </si>
+  <si>
+    <t>92856697Q</t>
+  </si>
+  <si>
+    <t>ekthor@email.com</t>
+  </si>
+  <si>
+    <t>Elkin Octavio Díaz</t>
+  </si>
+  <si>
+    <t>82430695Y</t>
+  </si>
+  <si>
+    <t>octavio@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +248,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,10 +281,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -186,7 +347,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,7 +382,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -406,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +663,244 @@
         <v>263</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -509,8 +908,23 @@
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
+    <hyperlink ref="C13" r:id="rId10"/>
+    <hyperlink ref="C14" r:id="rId11"/>
+    <hyperlink ref="C15" r:id="rId12"/>
+    <hyperlink ref="C16" r:id="rId13"/>
+    <hyperlink ref="C17" r:id="rId14"/>
+    <hyperlink ref="C18" r:id="rId15"/>
+    <hyperlink ref="C19" r:id="rId16"/>
+    <hyperlink ref="C20" r:id="rId17"/>
+    <hyperlink ref="C21" r:id="rId18"/>
+    <hyperlink ref="C22" r:id="rId19"/>
+    <hyperlink ref="C23" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>